<commit_message>
plano de aulas com bibliografia
</commit_message>
<xml_diff>
--- a/content/plano-de-aulas.xlsx
+++ b/content/plano-de-aulas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="83">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -42,112 +42,187 @@
     <t xml:space="preserve">Mutirão C</t>
   </si>
   <si>
+    <t xml:space="preserve">Exercícios no prairielearn (ref Kochan Caps 1 a 5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercícios no prairielearn (ref Kochan Caps 6e 10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercícios no prairielearn (ref Kochan caps 8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alocação de Memória Dinâmica + ADT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alunos implementam estrutura de dados simples para alocar matriz e acessar elementos (ref Kochan cap 16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reformular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Árvore Binária de Busca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introdução à árvores de busca binárias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercícios de simulação para introdução de árvores (ref Feofiloff cap 14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definição , inserção, visitação</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">implementações + atividades teóricas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(ref Feofiloff cap 14)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">implementações + atividades teóricas (ref Feofiloff cap 14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotações e remoção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementações + atividades teóricas (ref Feofiloff cap 15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balancear árvore torta (ordem ótima de inserção)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementações + atividades teóricas (ref Feofiloff cap 15 e Cormen cap 12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisão Geral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problemas leetcode para revisão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaliação docente + revisão pra prova + montar folha de consulta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intro a Grafos: ADT, componentes e ciclos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introdução a Grafos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluno usa ADT matriz para representar grafo e cria alguns grafos manualmente usando a ADT (ref Cormen cap 22.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluno usa ADT matriz ligada para representar grafo e cria alguns grafos manualmente usando a ADT (ref Cormen cap 22.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grafos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aula estúdio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Componentes Conexos, ciclos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluno implementa DFS para encontrar componentes conexos e ciclos.  (ref Cormen 22.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refazer testes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluno implementa DFS para encontrar componentes conexos e ciclos. (ref Cormen 22.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ordenação topológica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problema 1: compilação de projetos (ref Cormen 22.4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caminhos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFS + Fila (ref Cormen 10.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFS + Fila (ref Cormen 22.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aula estúdio (exercícios de busca em largura)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grafos com pesos: Dijkstra e caminhos mínimos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulação do algoritmo + implementação da ADT min-heap (ref Cormen 24.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aula estúdio (exercícios de código de caminhos mínimos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaliação docente + revisão pra prova + montar folha de consultao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exercícios no prairielearn</t>
   </si>
   <si>
-    <t xml:space="preserve">Alocação de Memória Dinâmica + ADT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Alunos implementam estrutura de dados simples para alocar matriz e acessar elementos</t>
   </si>
   <si>
-    <t xml:space="preserve">Reformular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Árvore Binária de Busca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introdução à árvores de busca binárias</t>
+    <t xml:space="preserve">Feriado</t>
   </si>
   <si>
     <t xml:space="preserve">Exercícios de simulação para introdução de árvores</t>
   </si>
   <si>
-    <t xml:space="preserve">Definição , inserção, visitação</t>
-  </si>
-  <si>
     <t xml:space="preserve">implementações + atividades teóricas</t>
   </si>
   <si>
-    <t xml:space="preserve">Rotações e remoção</t>
-  </si>
-  <si>
-    <t xml:space="preserve">balancear árvore torta (ordem ótima de inserção)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisão Geral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problemas leetcode para revisão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avaliação docente + revisão pra prova + montar folha de consultao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intro a Grafos: ADT, componentes e ciclos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introdução a Grafos </t>
+    <t xml:space="preserve">balancear árvore torta</t>
   </si>
   <si>
     <t xml:space="preserve">Aluno usa ADT matriz para representar grafo e cria alguns grafos manualmente usando a ADT</t>
   </si>
   <si>
-    <t xml:space="preserve">Grafos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aula estúdio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Componentes Conexos, ciclos</t>
+    <t xml:space="preserve">Revisão para prova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revisão pra prova + montar folha de consulta</t>
   </si>
   <si>
     <t xml:space="preserve">Aluno implementa DFS para encontrar componentes conexos e ciclos. </t>
   </si>
   <si>
-    <t xml:space="preserve">Refazer testes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ordenação topológica</t>
-  </si>
-  <si>
     <t xml:space="preserve">Problema 1: compilação de projetos</t>
   </si>
   <si>
-    <t xml:space="preserve">Caminhos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BFS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BFS + Fila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grafos com pesos: Dijkstra e caminhos mínimos</t>
+    <t xml:space="preserve">ADT Fila</t>
   </si>
   <si>
     <t xml:space="preserve">Simulação do algoritmo + implementação da ADT min-heap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feriado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">balancear árvore torta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revisão para prova</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revisão pra prova + montar folha de consulta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADT Fila</t>
   </si>
   <si>
     <t xml:space="preserve">FERIADO</t>
@@ -224,7 +299,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,6 +321,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -361,7 +442,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -377,6 +458,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -385,7 +470,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -422,10 +507,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -688,8 +769,8 @@
   </sheetPr>
   <dimension ref="A1:XFD31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D15" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -698,7 +779,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="30.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="49.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.71"/>
   </cols>
   <sheetData>
@@ -744,7 +825,7 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="XFD3" s="6"/>
     </row>
@@ -761,7 +842,7 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -773,14 +854,14 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -789,14 +870,14 @@
         <v>45524</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="10"/>
@@ -809,14 +890,14 @@
         <v>45527</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="10"/>
@@ -829,14 +910,14 @@
         <v>45531</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="10"/>
@@ -849,14 +930,14 @@
         <v>45534</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
-        <v>14</v>
+      <c r="E9" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -865,14 +946,14 @@
         <v>45538</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>14</v>
+      <c r="E10" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -881,14 +962,14 @@
         <v>45541</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="9" t="s">
-        <v>14</v>
+      <c r="E11" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="10"/>
@@ -901,14 +982,14 @@
         <v>45545</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -916,17 +997,17 @@
         <f aca="false">A11 +7</f>
         <v>45548</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>20</v>
+      <c r="B13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -938,17 +1019,17 @@
         <f aca="false">A12 + 7</f>
         <v>45552</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>20</v>
+      <c r="B14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -957,17 +1038,17 @@
         <v>45555</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -976,17 +1057,17 @@
         <v>45559</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -995,17 +1076,17 @@
         <v>45562</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1014,17 +1095,17 @@
         <v>45566</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="10"/>
@@ -1037,17 +1118,17 @@
         <v>45569</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>28</v>
+        <v>35</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="10"/>
@@ -1060,14 +1141,14 @@
         <v>45573</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1076,17 +1157,17 @@
         <v>45576</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1095,17 +1176,17 @@
         <v>45580</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>28</v>
+        <v>41</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="10"/>
@@ -1118,14 +1199,14 @@
         <v>45583</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1134,17 +1215,17 @@
         <v>45587</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>28</v>
+        <v>44</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="10"/>
@@ -1157,17 +1238,17 @@
         <v>45590</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>28</v>
+        <v>44</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="10"/>
@@ -1180,14 +1261,14 @@
         <v>45594</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="10"/>
@@ -1200,14 +1281,14 @@
         <v>45597</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="10"/>
@@ -1220,14 +1301,14 @@
         <v>45601</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1235,17 +1316,17 @@
         <f aca="false">A27 +7</f>
         <v>45604</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>36</v>
+      <c r="B29" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1253,17 +1334,17 @@
         <f aca="false">A28 + 7</f>
         <v>45608</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>36</v>
+      <c r="B30" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,8 +1372,8 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1304,17 +1385,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10"/>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1322,62 +1403,62 @@
       <c r="A2" s="6" t="n">
         <v>45327</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="10"/>
-      <c r="E2" s="14" t="s">
-        <v>6</v>
+      <c r="E2" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
         <v>45331</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>7</v>
+      <c r="C3" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="14" t="s">
-        <v>8</v>
+      <c r="E3" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="n">
+      <c r="A4" s="17" t="n">
         <f aca="false">A2 + 7</f>
         <v>45334</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="18"/>
+      <c r="B4" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
         <f aca="false">A3 +7</f>
         <v>45338</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>11</v>
+      <c r="B5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="14" t="s">
-        <v>12</v>
+      <c r="E5" s="15" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,15 +1466,15 @@
         <f aca="false">A4 + 7</f>
         <v>45341</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>13</v>
+      <c r="B6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="D6" s="10"/>
-      <c r="E6" s="14" t="s">
-        <v>14</v>
+      <c r="E6" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,15 +1482,15 @@
         <f aca="false">A5 +7</f>
         <v>45345</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>18</v>
+      <c r="B7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="14" t="s">
-        <v>25</v>
+      <c r="E7" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,15 +1498,15 @@
         <f aca="false">A6 + 7</f>
         <v>45348</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>15</v>
+      <c r="B8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="14" t="s">
-        <v>14</v>
+      <c r="E8" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1433,15 +1514,15 @@
         <f aca="false">A7 +7</f>
         <v>45352</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>18</v>
+      <c r="B9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="14" t="s">
-        <v>14</v>
+      <c r="E9" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1449,15 +1530,15 @@
         <f aca="false">A8 + 7</f>
         <v>45355</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>38</v>
+      <c r="B10" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="E10" s="14" t="s">
-        <v>14</v>
+      <c r="E10" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,15 +1546,15 @@
         <f aca="false">A9 +7</f>
         <v>45359</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>18</v>
+      <c r="B11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="14" t="s">
-        <v>14</v>
+      <c r="E11" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,15 +1562,15 @@
         <f aca="false">A10 + 7</f>
         <v>45362</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>22</v>
+      <c r="B12" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="D12" s="10"/>
-      <c r="E12" s="14" t="s">
-        <v>23</v>
+      <c r="E12" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,15 +1578,15 @@
         <f aca="false">A11 +7</f>
         <v>45366</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>18</v>
+      <c r="B13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="14" t="s">
-        <v>25</v>
+      <c r="E13" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1513,15 +1594,15 @@
         <f aca="false">A12 + 7</f>
         <v>45369</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>40</v>
+      <c r="B14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>56</v>
       </c>
       <c r="D14" s="10"/>
-      <c r="E14" s="14" t="s">
-        <v>40</v>
+      <c r="E14" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1529,17 +1610,17 @@
         <f aca="false">A13 +7</f>
         <v>45373</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>20</v>
+      <c r="B15" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1547,35 +1628,35 @@
         <f aca="false">A14 + 7</f>
         <v>45376</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>20</v>
+      <c r="B16" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="n">
+      <c r="A17" s="17" t="n">
         <f aca="false">A15 +7</f>
         <v>45380</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>37</v>
+      <c r="B17" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="I17" s="6"/>
     </row>
@@ -1584,15 +1665,15 @@
         <f aca="false">A16 + 7</f>
         <v>45383</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>22</v>
+      <c r="B18" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="D18" s="10"/>
-      <c r="E18" s="14" t="s">
-        <v>23</v>
+      <c r="E18" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,15 +1681,15 @@
         <f aca="false">A17 +7</f>
         <v>45387</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>18</v>
+      <c r="B19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D19" s="10"/>
-      <c r="E19" s="14" t="s">
-        <v>25</v>
+      <c r="E19" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="I19" s="6"/>
     </row>
@@ -1617,15 +1698,15 @@
         <f aca="false">A18 + 7</f>
         <v>45390</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="14" t="s">
+      <c r="B20" s="16" t="s">
         <v>26</v>
       </c>
+      <c r="C20" s="15" t="s">
+        <v>32</v>
+      </c>
       <c r="D20" s="10"/>
-      <c r="E20" s="14" t="s">
-        <v>27</v>
+      <c r="E20" s="15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1633,15 +1714,15 @@
         <f aca="false">A19 +7</f>
         <v>45394</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>18</v>
+      <c r="B21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D21" s="10"/>
-      <c r="E21" s="14" t="s">
-        <v>25</v>
+      <c r="E21" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1649,15 +1730,15 @@
         <f aca="false">A20 + 7</f>
         <v>45397</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>29</v>
+      <c r="B22" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="D22" s="10"/>
-      <c r="E22" s="14" t="s">
-        <v>30</v>
+      <c r="E22" s="15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,15 +1746,15 @@
         <f aca="false">A21 +7</f>
         <v>45401</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>18</v>
+      <c r="B23" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D23" s="10"/>
-      <c r="E23" s="14" t="s">
-        <v>25</v>
+      <c r="E23" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,15 +1762,15 @@
         <f aca="false">A22 + 7</f>
         <v>45404</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>32</v>
+      <c r="B24" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="D24" s="10"/>
-      <c r="E24" s="14" t="s">
-        <v>41</v>
+      <c r="E24" s="15" t="s">
+        <v>59</v>
       </c>
       <c r="I24" s="6"/>
     </row>
@@ -1698,15 +1779,15 @@
         <f aca="false">A23 +7</f>
         <v>45408</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>18</v>
+      <c r="B25" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D25" s="10"/>
-      <c r="E25" s="14" t="s">
-        <v>25</v>
+      <c r="E25" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,15 +1795,15 @@
         <f aca="false">A24 + 7</f>
         <v>45411</v>
       </c>
-      <c r="B26" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>34</v>
+      <c r="B26" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="D26" s="10"/>
-      <c r="E26" s="14" t="s">
-        <v>35</v>
+      <c r="E26" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1730,15 +1811,15 @@
         <f aca="false">A25 +7</f>
         <v>45415</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>18</v>
+      <c r="B27" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D27" s="10"/>
-      <c r="E27" s="14" t="s">
-        <v>25</v>
+      <c r="E27" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,51 +1827,51 @@
         <f aca="false">A26 + 7</f>
         <v>45418</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>18</v>
+      <c r="B28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="D28" s="10"/>
-      <c r="E28" s="14" t="s">
-        <v>25</v>
+      <c r="E28" s="15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16" t="n">
+      <c r="A29" s="17" t="n">
         <f aca="false">A27 +7</f>
         <v>45422</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>36</v>
+      <c r="B29" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16" t="n">
+      <c r="A30" s="17" t="n">
         <f aca="false">A28 + 7</f>
         <v>45425</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>36</v>
+      <c r="B30" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,8 +1899,8 @@
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1837,18 +1918,18 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="n">
+      <c r="A2" s="21" t="n">
         <v>45152</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1856,10 +1937,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="n">
+      <c r="A3" s="21" t="n">
         <v>45156</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1867,11 +1948,11 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="n">
+      <c r="A4" s="21" t="n">
         <f aca="false">A2 + 7</f>
         <v>45159</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1879,63 +1960,63 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="n">
+      <c r="A5" s="21" t="n">
         <f aca="false">A3 +7</f>
         <v>45163</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="n">
+      <c r="A6" s="21" t="n">
         <f aca="false">A4 + 7</f>
         <v>45166</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>21</v>
+      <c r="B6" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="n">
+      <c r="A7" s="21" t="n">
         <f aca="false">A5 +7</f>
         <v>45170</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>21</v>
+      <c r="B7" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" s="21" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="21" t="n">
         <f aca="false">A6 + 7</f>
         <v>45173</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>21</v>
+      <c r="B8" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1943,19 +2024,19 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="n">
+      <c r="A9" s="17" t="n">
         <f aca="false">A7 +7</f>
         <v>45177</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
@@ -1963,13 +2044,13 @@
         <v>45180</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1978,13 +2059,13 @@
         <v>45184</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,11 +2073,11 @@
         <f aca="false">A10 + 7</f>
         <v>45187</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>43</v>
+      <c r="B12" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,7 +2087,7 @@
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="25" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,7 +2097,7 @@
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="25" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,13 +2106,13 @@
         <v>45198</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="E15" s="1"/>
       <c r="G15" s="1"/>
@@ -2042,11 +2123,11 @@
         <f aca="false">A14 + 7</f>
         <v>45201</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>47</v>
+      <c r="B16" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2055,10 +2136,10 @@
         <v>45205</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2067,26 +2148,26 @@
         <v>45208</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="n">
+      <c r="A19" s="17" t="n">
         <f aca="false">A17 +7</f>
         <v>45212</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="n">
@@ -2094,10 +2175,10 @@
         <v>45215</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,10 +2187,10 @@
         <v>45219</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E21" s="1"/>
       <c r="G21" s="1"/>
@@ -2121,10 +2202,10 @@
         <v>45222</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,10 +2214,10 @@
         <v>45226</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2145,26 +2226,26 @@
         <v>45229</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="n">
+      <c r="A25" s="17" t="n">
         <f aca="false">A23 +7</f>
         <v>45233</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="n">
@@ -2172,10 +2253,10 @@
         <v>45236</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,23 +2266,23 @@
       </c>
       <c r="B27" s="24"/>
       <c r="C27" s="25" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F30" s="1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F31" s="1" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="G31" s="1" t="n">
         <v>17</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização do plano de aulas
</commit_message>
<xml_diff>
--- a/content/plano-de-aulas.xlsx
+++ b/content/plano-de-aulas.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="85">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -87,6 +87,21 @@
     <t xml:space="preserve">implementações + atividades teóricas (ref Feofiloff cap 15 e Cormen cap 12)</t>
   </si>
   <si>
+    <t xml:space="preserve">Intro a Grafos: ADT, componentes e ciclos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introdução a Grafos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definições básicas de grafos: vértices, arestas, grau, ciclos e componentes. (ref Cormen cap 22.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reformular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluno usa ADT matriz ligada para representar grafo e cria alguns grafos manualmente usando a ADT. Aluno cria matrizes de adjacências a partir de um desenho de um grafo (ref Cormen cap 22.1)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Revisão Geral</t>
   </si>
   <si>
@@ -99,88 +114,79 @@
     <t xml:space="preserve">PI</t>
   </si>
   <si>
-    <t xml:space="preserve">Intro a Grafos: ADT, componentes e ciclos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introdução a Grafos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aluno usa ADT matriz para representar grafo e cria alguns grafos manualmente usando a ADT (ref Cormen cap 22.1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reformular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aluno usa ADT matriz ligada para representar grafo e cria alguns grafos manualmente usando a ADT (ref Cormen cap 22.1)</t>
+    <t xml:space="preserve">Revisão pós-prova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comentários sobre os exercícios + introdução do próximo assunto. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Componentes Conexos, ciclos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluno implementa DFS para encontrar componentes conexos e ciclos.  (ref Cormen 22.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refazer testes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aluno implementa DFS para encontrar componentes conexos e ciclos. (ref Cormen 22.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ordenação topológica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problema 1: compilação de projetos (ref Cormen 22.4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caminhos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFS + Fila (ref Cormen 10.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFS + Fila (ref Cormen 22.2)</t>
   </si>
   <si>
     <t xml:space="preserve">Grafos</t>
   </si>
   <si>
+    <t xml:space="preserve">aula estúdio (exercícios de busca em largura)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grafos com pesos: Dijkstra e caminhos mínimos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulação do algoritmo + implementação da ADT min-heap (ref Cormen 24.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aula estúdio (exercícios de código de caminhos mínimos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avaliação docente + revisão pra prova + montar folha de consultao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercícios no prairielearn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alunos implementam estrutura de dados simples para alocar matriz e acessar elementos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feriado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercícios de simulação para introdução de árvores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implementações + atividades teóricas</t>
+  </si>
+  <si>
     <t xml:space="preserve">aula estúdio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Componentes Conexos, ciclos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aluno implementa DFS para encontrar componentes conexos e ciclos.  (ref Cormen 22.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refazer testes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aluno implementa DFS para encontrar componentes conexos e ciclos. (ref Cormen 22.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ordenação topológica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problema 1: compilação de projetos (ref Cormen 22.4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caminhos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BFS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BFS + Fila (ref Cormen 10.1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BFS + Fila (ref Cormen 22.2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aula estúdio (exercícios de busca em largura)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grafos com pesos: Dijkstra e caminhos mínimos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simulação do algoritmo + implementação da ADT min-heap (ref Cormen 24.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aula estúdio (exercícios de código de caminhos mínimos)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avaliação docente + revisão pra prova + montar folha de consultao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exercícios no prairielearn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alunos implementam estrutura de dados simples para alocar matriz e acessar elementos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feriado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exercícios de simulação para introdução de árvores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">implementações + atividades teóricas</t>
   </si>
   <si>
     <t xml:space="preserve">balancear árvore torta</t>
@@ -305,7 +311,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,14 +338,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF9999"/>
         <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
     <fill>
@@ -357,7 +369,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDE8CFF"/>
-        <bgColor rgb="FF9999FF"/>
+        <bgColor rgb="FFFF9999"/>
       </patternFill>
     </fill>
   </fills>
@@ -395,7 +407,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -440,63 +452,71 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -527,7 +547,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFF6F9D4"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -751,8 +771,8 @@
   </sheetPr>
   <dimension ref="A1:XFD31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="A15:F15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1000,106 +1020,102 @@
       <c r="E12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F12" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="54.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
         <f aca="false">A11 +7</f>
         <v>45548</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="0"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="G13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
         <f aca="false">A12 + 7</f>
         <v>45552</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
         <f aca="false">A13 +7</f>
         <v>45555</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>28</v>
-      </c>
+      <c r="B15" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="0"/>
+      <c r="G15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <f aca="false">A14 + 7</f>
         <v>45559</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
+      <c r="B16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>28</v>
-      </c>
+      <c r="C16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="0"/>
+      <c r="G16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
         <f aca="false">A15 +7</f>
         <v>45562</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>28</v>
+      <c r="F17" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1108,7 +1124,7 @@
         <v>45566</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>32</v>
@@ -1117,7 +1133,7 @@
       <c r="E18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="16" t="s">
         <v>34</v>
       </c>
       <c r="G18" s="7"/>
@@ -1131,7 +1147,7 @@
         <v>45569</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>32</v>
@@ -1140,7 +1156,7 @@
       <c r="E19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="16" t="s">
         <v>34</v>
       </c>
       <c r="G19" s="7"/>
@@ -1154,7 +1170,7 @@
         <v>45573</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>36</v>
@@ -1179,7 +1195,7 @@
       <c r="E21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1198,7 +1214,7 @@
       <c r="E22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="16" t="s">
         <v>34</v>
       </c>
       <c r="G22" s="7"/>
@@ -1212,14 +1228,14 @@
         <v>45583</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1231,13 +1247,13 @@
         <v>38</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>34</v>
       </c>
       <c r="G24" s="7"/>
@@ -1254,13 +1270,13 @@
         <v>38</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="16" t="s">
         <v>34</v>
       </c>
       <c r="G25" s="7"/>
@@ -1274,14 +1290,14 @@
         <v>45594</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="10"/>
@@ -1294,14 +1310,14 @@
         <v>45597</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="10"/>
@@ -1314,14 +1330,14 @@
         <v>45601</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1329,17 +1345,17 @@
         <f aca="false">A27 +7</f>
         <v>45604</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>47</v>
+      <c r="B29" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1347,17 +1363,17 @@
         <f aca="false">A28 + 7</f>
         <v>45608</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>47</v>
+      <c r="B30" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1386,7 +1402,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A15:F15 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1398,17 +1414,17 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="10"/>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1416,62 +1432,62 @@
       <c r="A2" s="7" t="n">
         <v>45327</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="10"/>
-      <c r="E2" s="15" t="s">
-        <v>48</v>
+      <c r="E2" s="17" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
         <v>45331</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="10"/>
-      <c r="E3" s="15" t="s">
-        <v>49</v>
+      <c r="E3" s="17" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="n">
+      <c r="A4" s="19" t="n">
         <f aca="false">A2 + 7</f>
         <v>45334</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="19"/>
+      <c r="B4" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="n">
         <f aca="false">A3 +7</f>
         <v>45338</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="17" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="10"/>
-      <c r="E5" s="15" t="s">
-        <v>51</v>
+      <c r="E5" s="17" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1479,15 +1495,15 @@
         <f aca="false">A4 + 7</f>
         <v>45341</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="10"/>
-      <c r="E6" s="15" t="s">
-        <v>52</v>
+      <c r="E6" s="17" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,15 +1511,15 @@
         <f aca="false">A5 +7</f>
         <v>45345</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>22</v>
+      <c r="C7" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="15" t="s">
-        <v>31</v>
+      <c r="E7" s="17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1511,15 +1527,15 @@
         <f aca="false">A6 + 7</f>
         <v>45348</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="15" t="s">
-        <v>52</v>
+      <c r="E8" s="17" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1527,15 +1543,15 @@
         <f aca="false">A7 +7</f>
         <v>45352</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>22</v>
+      <c r="C9" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="15" t="s">
-        <v>52</v>
+      <c r="E9" s="17" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1543,15 +1559,15 @@
         <f aca="false">A8 + 7</f>
         <v>45355</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1559,15 +1575,15 @@
         <f aca="false">A9 +7</f>
         <v>45359</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>22</v>
+      <c r="C11" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D11" s="10"/>
-      <c r="E11" s="15" t="s">
-        <v>52</v>
+      <c r="E11" s="17" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,15 +1591,15 @@
         <f aca="false">A10 + 7</f>
         <v>45362</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>26</v>
+      <c r="B12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="10"/>
-      <c r="E12" s="15" t="s">
-        <v>54</v>
+      <c r="E12" s="17" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,15 +1607,15 @@
         <f aca="false">A11 +7</f>
         <v>45366</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>22</v>
+      <c r="B13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="15" t="s">
-        <v>31</v>
+      <c r="E13" s="17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1607,15 +1623,15 @@
         <f aca="false">A12 + 7</f>
         <v>45369</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>56</v>
+      <c r="B14" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="D14" s="10"/>
-      <c r="E14" s="15" t="s">
-        <v>56</v>
+      <c r="E14" s="17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,17 +1639,17 @@
         <f aca="false">A13 +7</f>
         <v>45373</v>
       </c>
-      <c r="B15" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>24</v>
+      <c r="B15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1641,35 +1657,35 @@
         <f aca="false">A14 + 7</f>
         <v>45376</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>24</v>
+      <c r="B16" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="n">
+      <c r="A17" s="19" t="n">
         <f aca="false">A15 +7</f>
         <v>45380</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>50</v>
+      <c r="B17" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>51</v>
       </c>
       <c r="I17" s="7"/>
     </row>
@@ -1678,15 +1694,15 @@
         <f aca="false">A16 + 7</f>
         <v>45383</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>26</v>
+      <c r="B18" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>22</v>
       </c>
       <c r="D18" s="10"/>
-      <c r="E18" s="15" t="s">
-        <v>54</v>
+      <c r="E18" s="17" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,15 +1710,15 @@
         <f aca="false">A17 +7</f>
         <v>45387</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>22</v>
+      <c r="B19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D19" s="10"/>
-      <c r="E19" s="15" t="s">
-        <v>31</v>
+      <c r="E19" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="I19" s="7"/>
     </row>
@@ -1711,15 +1727,15 @@
         <f aca="false">A18 + 7</f>
         <v>45390</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="15" t="s">
+      <c r="B20" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="10"/>
-      <c r="E20" s="15" t="s">
-        <v>57</v>
+      <c r="E20" s="17" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,15 +1743,15 @@
         <f aca="false">A19 +7</f>
         <v>45394</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>22</v>
+      <c r="B21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D21" s="10"/>
-      <c r="E21" s="15" t="s">
-        <v>31</v>
+      <c r="E21" s="17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1743,15 +1759,15 @@
         <f aca="false">A20 + 7</f>
         <v>45397</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="15" t="s">
+      <c r="B22" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="10"/>
-      <c r="E22" s="15" t="s">
-        <v>58</v>
+      <c r="E22" s="17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1759,15 +1775,15 @@
         <f aca="false">A21 +7</f>
         <v>45401</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>22</v>
+      <c r="B23" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D23" s="10"/>
-      <c r="E23" s="15" t="s">
-        <v>31</v>
+      <c r="E23" s="17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,15 +1791,15 @@
         <f aca="false">A22 + 7</f>
         <v>45404</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="17" t="s">
         <v>39</v>
       </c>
       <c r="D24" s="10"/>
-      <c r="E24" s="15" t="s">
-        <v>59</v>
+      <c r="E24" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="I24" s="7"/>
     </row>
@@ -1792,15 +1808,15 @@
         <f aca="false">A23 +7</f>
         <v>45408</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>22</v>
+      <c r="B25" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D25" s="10"/>
-      <c r="E25" s="15" t="s">
-        <v>31</v>
+      <c r="E25" s="17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,15 +1824,15 @@
         <f aca="false">A24 + 7</f>
         <v>45411</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>43</v>
+      <c r="C26" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="D26" s="10"/>
-      <c r="E26" s="15" t="s">
-        <v>60</v>
+      <c r="E26" s="17" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1824,15 +1840,15 @@
         <f aca="false">A25 +7</f>
         <v>45415</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>22</v>
+      <c r="B27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D27" s="10"/>
-      <c r="E27" s="15" t="s">
-        <v>31</v>
+      <c r="E27" s="17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1840,51 +1856,51 @@
         <f aca="false">A26 + 7</f>
         <v>45418</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>22</v>
+      <c r="B28" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="D28" s="10"/>
-      <c r="E28" s="15" t="s">
-        <v>31</v>
+      <c r="E28" s="17" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17" t="n">
+      <c r="A29" s="19" t="n">
         <f aca="false">A27 +7</f>
         <v>45422</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>47</v>
+      <c r="B29" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="n">
+      <c r="A30" s="19" t="n">
         <f aca="false">A28 + 7</f>
         <v>45425</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>47</v>
+      <c r="B30" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1913,7 +1929,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A15:F15 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1931,18 +1947,18 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="n">
+      <c r="A2" s="23" t="n">
         <v>45152</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1950,10 +1966,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="n">
+      <c r="A3" s="23" t="n">
         <v>45156</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1961,11 +1977,11 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="n">
+      <c r="A4" s="23" t="n">
         <f aca="false">A2 + 7</f>
         <v>45159</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1973,63 +1989,63 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="n">
+      <c r="A5" s="23" t="n">
         <f aca="false">A3 +7</f>
         <v>45163</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="n">
+      <c r="A6" s="23" t="n">
         <f aca="false">A4 + 7</f>
         <v>45166</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>25</v>
+      <c r="B6" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="n">
+      <c r="A7" s="23" t="n">
         <f aca="false">A5 +7</f>
         <v>45170</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>25</v>
+      <c r="B7" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23" t="n">
         <f aca="false">A6 + 7</f>
         <v>45173</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>25</v>
+      <c r="B8" s="23" t="s">
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2037,19 +2053,19 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="n">
+      <c r="A9" s="19" t="n">
         <f aca="false">A7 +7</f>
         <v>45177</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="n">
@@ -2063,7 +2079,7 @@
         <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2075,10 +2091,10 @@
         <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2086,11 +2102,11 @@
         <f aca="false">A10 + 7</f>
         <v>45187</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>62</v>
+      <c r="C12" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2098,9 +2114,9 @@
         <f aca="false">A11 +7</f>
         <v>45191</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25" t="s">
-        <v>24</v>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,9 +2124,9 @@
         <f aca="false">A12 + 7</f>
         <v>45194</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25" t="s">
-        <v>24</v>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,13 +2135,13 @@
         <v>45198</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1"/>
       <c r="G15" s="1"/>
@@ -2136,11 +2152,11 @@
         <f aca="false">A14 + 7</f>
         <v>45201</v>
       </c>
-      <c r="B16" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>66</v>
+      <c r="B16" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2149,10 +2165,10 @@
         <v>45205</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2161,26 +2177,26 @@
         <v>45208</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17" t="n">
+      <c r="A19" s="19" t="n">
         <f aca="false">A17 +7</f>
         <v>45212</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="n">
@@ -2188,10 +2204,10 @@
         <v>45215</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2200,10 +2216,10 @@
         <v>45219</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E21" s="1"/>
       <c r="G21" s="1"/>
@@ -2215,10 +2231,10 @@
         <v>45222</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2227,10 +2243,10 @@
         <v>45226</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2239,26 +2255,26 @@
         <v>45229</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17" t="n">
+      <c r="A25" s="19" t="n">
         <f aca="false">A23 +7</f>
         <v>45233</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="n">
@@ -2266,36 +2282,36 @@
         <v>45236</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="24" t="n">
+      <c r="A27" s="26" t="n">
         <f aca="false">A25 +7</f>
         <v>45240</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25" t="s">
-        <v>47</v>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F30" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F31" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G31" s="1" t="n">
         <v>17</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>